<commit_message>
wrote hypsometry stuff, fortran commit
</commit_message>
<xml_diff>
--- a/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
+++ b/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>depth</t>
   </si>
@@ -124,7 +124,7 @@
     <t>OUR Anders High</t>
   </si>
   <si>
-    <t>JO2 from paper (eq. 16)</t>
+    <t>Fraction of total</t>
   </si>
   <si>
     <t>OMEN</t>
@@ -182,6 +182,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -203,12 +204,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -219,8 +222,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -299,7 +301,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -601,11 +603,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88332993"/>
-        <c:axId val="3333967"/>
+        <c:axId val="22734102"/>
+        <c:axId val="19142566"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88332993"/>
+        <c:axId val="22734102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,11 +623,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3333967"/>
+        <c:crossAx val="19142566"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3333967"/>
+        <c:axId val="19142566"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -650,7 +652,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88332993"/>
+        <c:crossAx val="22734102"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -663,6 +665,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -685,7 +689,395 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart162.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>rate Fe red</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"exponential"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exponential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="666699"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="666699"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>exponential!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>89.6908203872887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.8537071093311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.3625242918782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.8160678720006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.93288575140178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.123403969229771</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"linear"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>linear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="993366"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="993366"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>linear!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>76.4442340767933</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.8518175958458</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.9572589474022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.3976979843909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.933770521939</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.2777936214685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>linear!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"no"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="99cc00"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="99cc00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>no!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3237456245636E-007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.73617866144958E-007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8643376671461E-007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.49892067269166E-007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.26312960937686E-007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.20473261085559E-007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>no!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="39324922"/>
+        <c:axId val="62500977"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="39324922"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="62500977"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="62500977"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="39324922"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="808080"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -987,11 +1379,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60391561"/>
-        <c:axId val="6991759"/>
+        <c:axId val="66747752"/>
+        <c:axId val="66380642"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60391561"/>
+        <c:axId val="66747752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,11 +1399,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6991759"/>
+        <c:crossAx val="66380642"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6991759"/>
+        <c:axId val="66380642"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1036,7 +1428,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60391561"/>
+        <c:crossAx val="66747752"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1049,6 +1441,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1071,7 +1465,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart163.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1373,11 +1767,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88909149"/>
-        <c:axId val="68732331"/>
+        <c:axId val="33008207"/>
+        <c:axId val="28659675"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88909149"/>
+        <c:axId val="33008207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1393,11 +1787,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68732331"/>
+        <c:crossAx val="28659675"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68732331"/>
+        <c:axId val="28659675"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1422,7 +1816,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88909149"/>
+        <c:crossAx val="33008207"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1435,6 +1829,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1457,7 +1853,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart164.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1759,11 +2155,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83497304"/>
-        <c:axId val="24105996"/>
+        <c:axId val="44202044"/>
+        <c:axId val="46886918"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83497304"/>
+        <c:axId val="44202044"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,11 +2175,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24105996"/>
+        <c:crossAx val="46886918"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24105996"/>
+        <c:axId val="46886918"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1808,7 +2204,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83497304"/>
+        <c:crossAx val="44202044"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1821,6 +2217,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1843,7 +2241,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart165.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2145,11 +2543,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92419434"/>
-        <c:axId val="84437575"/>
+        <c:axId val="14360733"/>
+        <c:axId val="53912267"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92419434"/>
+        <c:axId val="14360733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,11 +2563,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84437575"/>
+        <c:crossAx val="53912267"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84437575"/>
+        <c:axId val="53912267"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2194,7 +2592,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92419434"/>
+        <c:crossAx val="14360733"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2207,6 +2605,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2229,7 +2629,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart166.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2531,11 +2931,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85969172"/>
-        <c:axId val="557922"/>
+        <c:axId val="4274535"/>
+        <c:axId val="1147902"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85969172"/>
+        <c:axId val="4274535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2551,11 +2951,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="557922"/>
+        <c:crossAx val="1147902"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="557922"/>
+        <c:axId val="1147902"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2580,7 +2980,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85969172"/>
+        <c:crossAx val="4274535"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2593,6 +2993,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2615,7 +3017,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart167.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2917,11 +3319,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="98048569"/>
-        <c:axId val="48759292"/>
+        <c:axId val="92085717"/>
+        <c:axId val="18341732"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98048569"/>
+        <c:axId val="92085717"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2937,11 +3339,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48759292"/>
+        <c:crossAx val="18341732"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48759292"/>
+        <c:axId val="18341732"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2966,7 +3368,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98048569"/>
+        <c:crossAx val="92085717"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2979,6 +3381,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3001,7 +3405,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart168.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3303,11 +3707,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72037730"/>
-        <c:axId val="96240416"/>
+        <c:axId val="77929042"/>
+        <c:axId val="71260829"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72037730"/>
+        <c:axId val="77929042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3323,11 +3727,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96240416"/>
+        <c:crossAx val="71260829"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96240416"/>
+        <c:axId val="71260829"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3352,7 +3756,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72037730"/>
+        <c:crossAx val="77929042"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3365,6 +3769,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3387,7 +3793,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart169.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3689,11 +4095,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82327859"/>
-        <c:axId val="42275296"/>
+        <c:axId val="48343079"/>
+        <c:axId val="42241589"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82327859"/>
+        <c:axId val="48343079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3709,11 +4115,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42275296"/>
+        <c:crossAx val="42241589"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42275296"/>
+        <c:axId val="42241589"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3738,7 +4144,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82327859"/>
+        <c:crossAx val="48343079"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3751,392 +4157,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:solidFill>
-        <a:srgbClr val="808080"/>
-      </a:solidFill>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart170.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>rate Fe red</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"exponential"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>exponential</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="666699"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="666699"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>exponential!$L$2:$L$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>89.6908203872887</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80.8537071093311</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41.3625242918782</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.8160678720006</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.93288575140178</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.123403969229771</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"linear"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>linear</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="993366"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="993366"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>linear!$M$2:$M$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>76.4442340767933</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80.8518175958458</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62.9572589474022</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59.3976979843909</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39.933770521939</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18.2777936214685</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"no"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>no</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="99cc00"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="99cc00"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>no!$M$2:$M$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.3237456245636E-007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.73617866144958E-007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8643376671461E-007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.49892067269166E-007</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.26312960937686E-007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.20473261085559E-007</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="76473192"/>
-        <c:axId val="10610516"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="76473192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="808080"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="10610516"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="10610516"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="808080"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="808080"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="76473192"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4164,15 +4186,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>198360</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:colOff>225360</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>519120</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:colOff>545760</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4180,8 +4202,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="198360" y="8991000"/>
-        <a:ext cx="5165640" cy="2912400"/>
+        <a:off x="225360" y="8909640"/>
+        <a:ext cx="5073840" cy="2912040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4194,15 +4216,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:colOff>505800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:colOff>186480</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4210,8 +4232,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6398640" y="8981640"/>
-        <a:ext cx="5335920" cy="2912400"/>
+        <a:off x="6334200" y="8900280"/>
+        <a:ext cx="5221080" cy="2912040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4224,15 +4246,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:colOff>27000</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>348480</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:colOff>375120</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4240,8 +4262,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="12079800"/>
-        <a:ext cx="7545960" cy="2790720"/>
+        <a:off x="27000" y="11998440"/>
+        <a:ext cx="7408440" cy="2790360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4254,15 +4276,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:colOff>361080</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>681480</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4270,8 +4292,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8170560" y="12027600"/>
-        <a:ext cx="5772600" cy="2767320"/>
+        <a:off x="8037360" y="11946240"/>
+        <a:ext cx="5703840" cy="2766960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4284,15 +4306,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>599040</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:colOff>626040</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>596880</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:colOff>623520</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4300,8 +4322,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12173760" y="8958240"/>
-        <a:ext cx="5419440" cy="2743560"/>
+        <a:off x="11994840" y="8876880"/>
+        <a:ext cx="5396400" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4314,15 +4336,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:colOff>27000</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>320400</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:colOff>347040</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4330,8 +4352,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="15230160"/>
-        <a:ext cx="5165280" cy="2743200"/>
+        <a:off x="27000" y="15148800"/>
+        <a:ext cx="5073480" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4344,15 +4366,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>150120</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:colOff>177120</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>470160</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:colOff>496800</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4360,8 +4382,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6069960" y="15125040"/>
-        <a:ext cx="5040720" cy="2743560"/>
+        <a:off x="6005520" y="15043680"/>
+        <a:ext cx="4925880" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4374,15 +4396,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>50400</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:colOff>77400</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>861840</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:colOff>888480</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4390,8 +4412,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11625120" y="15153480"/>
-        <a:ext cx="7363080" cy="2743560"/>
+        <a:off x="11446200" y="15072120"/>
+        <a:ext cx="7340040" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4404,15 +4426,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:colOff>176400</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>470160</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>496800</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4420,8 +4442,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="149400" y="18201600"/>
-        <a:ext cx="5165640" cy="2743200"/>
+        <a:off x="176400" y="18120240"/>
+        <a:ext cx="5073840" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4434,15 +4456,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>150120</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:colOff>177120</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>470160</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>496800</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4450,8 +4472,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6069960" y="18201600"/>
-        <a:ext cx="5040720" cy="2743200"/>
+        <a:off x="6005520" y="18120240"/>
+        <a:ext cx="4925880" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4472,16 +4494,19 @@
   <dimension ref="A1:AD69"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.8163265306122"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.234693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.8163265306122"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2397959183673"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.234693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.219387755102"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.7602040816327"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.515306122449"/>
@@ -4492,6 +4517,7 @@
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.219387755102"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4626,7 +4652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>500</v>
       </c>
@@ -4960,13 +4986,13 @@
         <v>402.672618553322</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>100</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">646*(1/(500/B2-1))</f>
-        <v>415.010011852173</v>
+        <f aca="false">B2/G2</f>
+        <v>0.383476645926384</v>
       </c>
       <c r="Q10" s="0" t="n">
         <v>200</v>
@@ -5015,13 +5041,13 @@
         <v>315.207357868718</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>200</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">646*(1/(500/B3-1))</f>
-        <v>358.766437545991</v>
+        <f aca="false">B3/G3</f>
+        <v>0.382296051231655</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>500</v>
@@ -5070,13 +5096,13 @@
         <v>264.029552200547</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>500</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">646*(1/(500/B4-1))</f>
-        <v>232.085236926459</v>
+        <f aca="false">B4/G4</f>
+        <v>0.370179724892518</v>
       </c>
       <c r="Q12" s="0" t="n">
         <v>1000</v>
@@ -5125,13 +5151,13 @@
         <v>202.665702439887</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="B13" s="0" t="n">
-        <f aca="false">646*(1/(500/B5-1))</f>
-        <v>138.852889172965</v>
+        <f aca="false">B5/G5</f>
+        <v>0.387973280268588</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>2000</v>
@@ -5180,13 +5206,13 @@
         <v>119.367924489393</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="B14" s="0" t="n">
-        <f aca="false">646*(1/(500/B6-1))</f>
-        <v>68.2424505494995</v>
+        <f aca="false">B6/G6</f>
+        <v>0.51368396704109</v>
       </c>
       <c r="Q14" s="0" t="n">
         <v>3500</v>
@@ -5216,7 +5242,7 @@
       </c>
       <c r="Y14" s="2" t="n">
         <f aca="false">B7+X14</f>
-        <v>67.5765897195784</v>
+        <v>67.5765897195783</v>
       </c>
       <c r="Z14" s="0" t="n">
         <f aca="false">Z$4*((1-Z$5)*EXP(-Z$6*Q14)+Z$5*EXP(-Z$7*Q14))</f>
@@ -5235,13 +5261,13 @@
         <v>53.934328096248</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>3500</v>
       </c>
       <c r="B15" s="0" t="n">
-        <f aca="false">646*(1/(500/B7-1))</f>
-        <v>27.5782720930062</v>
+        <f aca="false">B7/G7</f>
+        <v>0.842447243033926</v>
       </c>
       <c r="Q15" s="0" t="n">
         <v>5000</v>
@@ -5290,13 +5316,13 @@
         <v>24.3625285793591</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="B16" s="0" t="n">
-        <f aca="false">646*(1/(500/B8-1))</f>
-        <v>9.08374397343126</v>
+        <f aca="false">B8/G8</f>
+        <v>1.09530320108985</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6139,7 +6165,186 @@
         <v>-0.000175158673674342</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <f aca="false">P31/Q31</f>
+        <v>0.992200635155694</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">B31/SUM(B31:D31)</f>
+        <v>0.989711128534426</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">E31/$H31</f>
+        <v>3.22072747263573E-005</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">F31/$H31</f>
+        <v>0.00293541427134572</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">G31/$H31</f>
+        <v>0.997032378453928</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <f aca="false">P32/Q32</f>
+        <v>0.991697541045026</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">B32/SUM(B32:D32)</f>
+        <v>0.987784844336868</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">E32/$H32</f>
+        <v>3.4610716243188E-005</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">F32/$H32</f>
+        <v>0.00321024441073962</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">G32/$H32</f>
+        <v>0.996755144873019</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <f aca="false">P33/Q33</f>
+        <v>0.985281016241932</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">B33/SUM(B33:D33)</f>
+        <v>0.976912822944023</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">E33/$H33</f>
+        <v>7.9480301805627E-005</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <f aca="false">F33/$H33</f>
+        <v>0.00558988220910321</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">G33/$H33</f>
+        <v>0.994330637489095</v>
+      </c>
+      <c r="P42" s="0" t="n">
+        <f aca="false">P34/Q34</f>
+        <v>0.978764496293136</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <f aca="false">B34/SUM(B34:D34)</f>
+        <v>0.964770674719555</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">E34/$H34</f>
+        <v>0.000138135918928745</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <f aca="false">F34/$H34</f>
+        <v>0.00832979835429118</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">G34/$H34</f>
+        <v>0.991532065726777</v>
+      </c>
+      <c r="P43" s="0" t="n">
+        <f aca="false">P35/Q35</f>
+        <v>0.948561699154825</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">B35/SUM(B35:D35)</f>
+        <v>0.938131681469408</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">E35/$H35</f>
+        <v>0.000646834837589846</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">F35/$H35</f>
+        <v>0.0179710786526344</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">G35/$H35</f>
+        <v>0.981382086509776</v>
+      </c>
+      <c r="P44" s="0" t="n">
+        <f aca="false">P36/Q36</f>
+        <v>0.738388759665891</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>3500</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <f aca="false">B36/SUM(B36:D36)</f>
+        <v>0.909300756722832</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">E36/$H36</f>
+        <v>0.011948964156142</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">F36/$H36</f>
+        <v>0.0628176998296365</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">G36/$H36</f>
+        <v>0.925233336014221</v>
+      </c>
+      <c r="P45" s="0" t="n">
+        <f aca="false">P37/Q37</f>
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">B37/SUM(B37:D37)</f>
+        <v>1.09921671058399</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">E37/$H37</f>
+        <v>1</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">F37/$H37</f>
+        <v>-0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">G37/$H37</f>
+        <v>-0</v>
+      </c>
+    </row>
     <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -6166,6 +6371,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6494,6 +6702,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
LateX: produced and described Thullner hypsometry plot
</commit_message>
<xml_diff>
--- a/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
+++ b/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="843" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="exponential" sheetId="1" state="visible" r:id="rId2"/>
@@ -177,12 +177,11 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -204,25 +203,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -338,7 +330,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -362,9 +354,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$B$2:$B$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -394,7 +415,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -428,7 +449,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -452,9 +473,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$B$2:$B$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -484,7 +534,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -518,7 +568,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -542,9 +592,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$B$2:$B$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -574,7 +653,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -603,11 +682,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="22734102"/>
-        <c:axId val="19142566"/>
+        <c:axId val="89653051"/>
+        <c:axId val="39061037"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22734102"/>
+        <c:axId val="89653051"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,11 +702,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19142566"/>
+        <c:crossAx val="39061037"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19142566"/>
+        <c:axId val="39061037"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -652,7 +731,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22734102"/>
+        <c:crossAx val="89653051"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -726,7 +805,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -750,9 +829,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$L$2:$L$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -782,7 +890,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -816,7 +924,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -840,9 +948,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$M$2:$M$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -872,7 +1009,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -906,7 +1043,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -930,9 +1067,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$M$2:$M$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -962,7 +1128,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -991,11 +1157,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="39324922"/>
-        <c:axId val="62500977"/>
+        <c:axId val="73841018"/>
+        <c:axId val="82291444"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39324922"/>
+        <c:axId val="73841018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,11 +1177,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62500977"/>
+        <c:crossAx val="82291444"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62500977"/>
+        <c:axId val="82291444"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1040,7 +1206,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39324922"/>
+        <c:crossAx val="73841018"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1114,7 +1280,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1138,9 +1304,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$C$2:$C$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1170,7 +1365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1204,7 +1399,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1228,9 +1423,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$C$2:$C$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1260,7 +1484,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1294,7 +1518,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1318,9 +1542,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$C$2:$C$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1350,7 +1603,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1379,11 +1632,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="66747752"/>
-        <c:axId val="66380642"/>
+        <c:axId val="88547780"/>
+        <c:axId val="3464580"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66747752"/>
+        <c:axId val="88547780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,11 +1652,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66380642"/>
+        <c:crossAx val="3464580"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66380642"/>
+        <c:axId val="3464580"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1428,7 +1681,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66747752"/>
+        <c:crossAx val="88547780"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1502,7 +1755,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1526,9 +1779,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$D$2:$D$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1558,7 +1840,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1592,7 +1874,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1616,9 +1898,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$D$2:$D$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1648,7 +1959,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1682,7 +1993,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1706,9 +2017,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$D$2:$D$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1738,7 +2078,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1767,11 +2107,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="33008207"/>
-        <c:axId val="28659675"/>
+        <c:axId val="74374968"/>
+        <c:axId val="24392565"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33008207"/>
+        <c:axId val="74374968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,11 +2127,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28659675"/>
+        <c:crossAx val="24392565"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="28659675"/>
+        <c:axId val="24392565"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1816,7 +2156,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33008207"/>
+        <c:crossAx val="74374968"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1890,7 +2230,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1914,9 +2254,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$E$2:$E$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1946,7 +2315,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1980,7 +2349,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2004,9 +2373,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$E$2:$E$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2036,7 +2434,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2070,7 +2468,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2094,9 +2492,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$E$2:$E$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2126,7 +2553,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2155,11 +2582,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="44202044"/>
-        <c:axId val="46886918"/>
+        <c:axId val="31197525"/>
+        <c:axId val="70304808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44202044"/>
+        <c:axId val="31197525"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,11 +2602,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46886918"/>
+        <c:crossAx val="70304808"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46886918"/>
+        <c:axId val="70304808"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2204,7 +2631,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44202044"/>
+        <c:crossAx val="31197525"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2278,7 +2705,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2302,9 +2729,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$F$2:$F$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2334,7 +2790,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2368,7 +2824,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2392,9 +2848,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$F$2:$F$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2424,7 +2909,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2458,7 +2943,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2482,9 +2967,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$F$2:$F$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2514,7 +3028,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2543,11 +3057,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="14360733"/>
-        <c:axId val="53912267"/>
+        <c:axId val="64962107"/>
+        <c:axId val="23166312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14360733"/>
+        <c:axId val="64962107"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,11 +3077,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53912267"/>
+        <c:crossAx val="23166312"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53912267"/>
+        <c:axId val="23166312"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2592,7 +3106,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14360733"/>
+        <c:crossAx val="64962107"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2666,7 +3180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2690,9 +3204,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$H$2:$H$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2722,7 +3265,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2756,7 +3299,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2780,9 +3323,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$I$2:$I$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2812,7 +3384,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2846,7 +3418,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2870,9 +3442,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$I$2:$I$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2902,7 +3503,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2931,11 +3532,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="4274535"/>
-        <c:axId val="1147902"/>
+        <c:axId val="88210856"/>
+        <c:axId val="16750046"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4274535"/>
+        <c:axId val="88210856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,11 +3552,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1147902"/>
+        <c:crossAx val="16750046"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1147902"/>
+        <c:axId val="16750046"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2980,7 +3581,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4274535"/>
+        <c:crossAx val="88210856"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3054,7 +3655,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3078,9 +3679,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$I$2:$I$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3110,7 +3740,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3144,7 +3774,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3168,9 +3798,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$J$2:$J$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3200,7 +3859,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3234,7 +3893,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3258,9 +3917,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$J$2:$J$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3290,7 +3978,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3319,11 +4007,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92085717"/>
-        <c:axId val="18341732"/>
+        <c:axId val="93723009"/>
+        <c:axId val="50377251"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92085717"/>
+        <c:axId val="93723009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3339,11 +4027,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18341732"/>
+        <c:crossAx val="50377251"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18341732"/>
+        <c:axId val="50377251"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3368,7 +4056,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92085717"/>
+        <c:crossAx val="93723009"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3442,7 +4130,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3466,9 +4154,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$J$2:$J$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3498,7 +4215,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3532,7 +4249,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3556,9 +4273,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$K$2:$K$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3588,7 +4334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3622,7 +4368,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3646,9 +4392,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$K$2:$K$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3678,7 +4453,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3707,11 +4482,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77929042"/>
-        <c:axId val="71260829"/>
+        <c:axId val="28115020"/>
+        <c:axId val="11878815"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77929042"/>
+        <c:axId val="28115020"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3727,11 +4502,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="71260829"/>
+        <c:crossAx val="11878815"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71260829"/>
+        <c:axId val="11878815"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3756,7 +4531,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77929042"/>
+        <c:crossAx val="28115020"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3830,7 +4605,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"exponential"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3854,9 +4629,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>exponential!$K$2:$K$8</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3886,7 +4690,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exponential!$A$2:$A$8</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3920,7 +4724,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>"linear"</c:f>
+              <c:f>label 3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3944,9 +4748,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>linear!$L$2:$L$8</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3976,7 +4809,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>linear!$A$2:$A$8</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4010,7 +4843,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>"no"</c:f>
+              <c:f>label 5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4034,9 +4867,38 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:smooth val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>no!$L$2:$L$8</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4066,7 +4928,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>no!$A$2:$A$8</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4095,11 +4957,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="48343079"/>
-        <c:axId val="42241589"/>
+        <c:axId val="1493159"/>
+        <c:axId val="71375494"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48343079"/>
+        <c:axId val="1493159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4115,11 +4977,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42241589"/>
+        <c:crossAx val="71375494"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42241589"/>
+        <c:axId val="71375494"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4144,7 +5006,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48343079"/>
+        <c:crossAx val="1493159"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4186,15 +5048,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>225360</xdr:colOff>
+      <xdr:colOff>252360</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>545760</xdr:colOff>
+      <xdr:colOff>572400</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4202,8 +5064,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="225360" y="8909640"/>
-        <a:ext cx="5073840" cy="2912040"/>
+        <a:off x="252360" y="8900640"/>
+        <a:ext cx="5073480" cy="2888280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4216,15 +5078,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>505800</xdr:colOff>
+      <xdr:colOff>533520</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>186480</xdr:colOff>
+      <xdr:colOff>213840</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4232,8 +5094,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6334200" y="8900280"/>
-        <a:ext cx="5221080" cy="2912040"/>
+        <a:off x="6361920" y="8891280"/>
+        <a:ext cx="5220720" cy="2888280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4246,15 +5108,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>375120</xdr:colOff>
+      <xdr:colOff>402480</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4262,8 +5124,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="27000" y="11998440"/>
-        <a:ext cx="7408440" cy="2790360"/>
+        <a:off x="54000" y="11989440"/>
+        <a:ext cx="7408800" cy="2767320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4276,15 +5138,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>361080</xdr:colOff>
+      <xdr:colOff>388800</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>681480</xdr:colOff>
+      <xdr:colOff>708840</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4292,8 +5154,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8037360" y="11946240"/>
-        <a:ext cx="5703840" cy="2766960"/>
+        <a:off x="8065080" y="11937240"/>
+        <a:ext cx="5703480" cy="2743920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4306,15 +5168,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>626040</xdr:colOff>
+      <xdr:colOff>653760</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
+      <xdr:colOff>650160</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4322,8 +5184,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11994840" y="8876880"/>
-        <a:ext cx="5396400" cy="2743200"/>
+        <a:off x="12022560" y="8867880"/>
+        <a:ext cx="5395320" cy="2720160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4336,15 +5198,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:colOff>54000</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>347040</xdr:colOff>
+      <xdr:colOff>373680</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4352,8 +5214,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="27000" y="15148800"/>
-        <a:ext cx="5073480" cy="2742840"/>
+        <a:off x="54000" y="15132960"/>
+        <a:ext cx="5073120" cy="2726640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4366,15 +5228,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>177120</xdr:colOff>
+      <xdr:colOff>204840</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>496800</xdr:colOff>
+      <xdr:colOff>524160</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4382,8 +5244,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6005520" y="15043680"/>
-        <a:ext cx="4925880" cy="2743200"/>
+        <a:off x="6033240" y="15034680"/>
+        <a:ext cx="4925520" cy="2720160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4396,15 +5258,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>77400</xdr:colOff>
+      <xdr:colOff>105120</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>888480</xdr:colOff>
+      <xdr:colOff>915840</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4412,8 +5274,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11446200" y="15072120"/>
-        <a:ext cx="7340040" cy="2743200"/>
+        <a:off x="11473920" y="15063120"/>
+        <a:ext cx="7339680" cy="2720160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4426,15 +5288,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>176400</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>496800</xdr:colOff>
+      <xdr:colOff>523440</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4442,8 +5304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="176400" y="18120240"/>
-        <a:ext cx="5073840" cy="2742840"/>
+        <a:off x="203400" y="18111240"/>
+        <a:ext cx="5073480" cy="2719800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4456,15 +5318,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>177120</xdr:colOff>
+      <xdr:colOff>204840</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>496800</xdr:colOff>
+      <xdr:colOff>524160</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4472,8 +5334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6005520" y="18120240"/>
-        <a:ext cx="4925880" cy="2742840"/>
+        <a:off x="6033240" y="18111240"/>
+        <a:ext cx="4925520" cy="2719800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4494,7 +5356,7 @@
   <dimension ref="A1:AD69"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="U29" activeCellId="0" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4861,7 +5723,7 @@
         <v>0.00053</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>5000</v>
       </c>
@@ -5230,7 +6092,7 @@
       </c>
       <c r="U14" s="2" t="n">
         <f aca="false">B7+T14</f>
-        <v>44.7578676524628</v>
+        <v>44.7578676524627</v>
       </c>
       <c r="W14" s="0" t="n">
         <f aca="false">W$4*((1-W$5)*EXP(-W$6*Q14)+W$5*EXP(-W$7*Q14))</f>
@@ -6263,7 +7125,7 @@
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">F34/$H34</f>
-        <v>0.00832979835429118</v>
+        <v>0.00832979835429117</v>
       </c>
       <c r="G43" s="0" t="n">
         <f aca="false">G34/$H34</f>
@@ -6372,7 +7234,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6703,7 +7569,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
LaTeX: Discussion: edited hypsometry section + started table in the methodology for it
</commit_message>
<xml_diff>
--- a/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
+++ b/Observations/Thullner_2009/ThullnerGcubed2009 Fluxes-rates.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="66">
   <si>
     <t>depth</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>rate-feoh3</t>
+  </si>
+  <si>
+    <t>TOTAL RATE</t>
   </si>
   <si>
     <t>POC flux calc</t>
@@ -130,6 +133,9 @@
     <t>Fraction of total</t>
   </si>
   <si>
+    <t>100/5000</t>
+  </si>
+  <si>
     <t>OMEN</t>
   </si>
   <si>
@@ -146,6 +152,9 @@
   </si>
   <si>
     <t>Gamma=0.05; gammaH2S=0.05;</t>
+  </si>
+  <si>
+    <t>FRACTIONS</t>
   </si>
   <si>
     <t>Gamma=0.95; gammaH2S=0.95; O2=10, NO3=80 +  + N:C = 0.067  east Pacific (Bohlen et al. 2012)</t>
@@ -400,7 +409,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,7 +449,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -742,11 +751,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="30721324"/>
-        <c:axId val="2374688"/>
+        <c:axId val="77633389"/>
+        <c:axId val="34272159"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30721324"/>
+        <c:axId val="77633389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,11 +771,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2374688"/>
+        <c:crossAx val="34272159"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2374688"/>
+        <c:axId val="34272159"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -791,7 +800,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30721324"/>
+        <c:crossAx val="77633389"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -828,7 +837,395 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>rate Fe red</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exponential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="666699"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="666699"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>89.6908203872887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.8537071093311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.3625242918782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.8160678720006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.93288575140178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.123403969229771</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>linear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="993366"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="993366"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>76.4442340767933</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.8518175958458</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.9572589474022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.3976979843909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.933770521939</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.2777936214685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="99cc00"/>
+            </a:solidFill>
+            <a:ln w="25200">
+              <a:solidFill>
+                <a:srgbClr val="99cc00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3237456245636E-007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.73617866144958E-007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8643376671461E-007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.49892067269166E-007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.26312960937686E-007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.20473261085559E-007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="65394138"/>
+        <c:axId val="7139299"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="65394138"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="7139299"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="7139299"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="65394138"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="808080"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1130,11 +1527,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55113725"/>
-        <c:axId val="62522236"/>
+        <c:axId val="20323180"/>
+        <c:axId val="10724408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55113725"/>
+        <c:axId val="20323180"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,11 +1547,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62522236"/>
+        <c:crossAx val="10724408"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62522236"/>
+        <c:axId val="10724408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1179,7 +1576,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55113725"/>
+        <c:crossAx val="20323180"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1216,7 +1613,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1518,11 +1915,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="3814486"/>
-        <c:axId val="28655873"/>
+        <c:axId val="72426303"/>
+        <c:axId val="57501112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3814486"/>
+        <c:axId val="72426303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,11 +1935,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28655873"/>
+        <c:crossAx val="57501112"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="28655873"/>
+        <c:axId val="57501112"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1567,7 +1964,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3814486"/>
+        <c:crossAx val="72426303"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1604,7 +2001,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1906,11 +2303,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="84328007"/>
-        <c:axId val="75579734"/>
+        <c:axId val="23951193"/>
+        <c:axId val="49303304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84328007"/>
+        <c:axId val="23951193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,11 +2323,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75579734"/>
+        <c:crossAx val="49303304"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75579734"/>
+        <c:axId val="49303304"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1955,7 +2352,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84328007"/>
+        <c:crossAx val="23951193"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1992,7 +2389,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2294,11 +2691,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="13500643"/>
-        <c:axId val="75328291"/>
+        <c:axId val="79649927"/>
+        <c:axId val="912690"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13500643"/>
+        <c:axId val="79649927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2314,11 +2711,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75328291"/>
+        <c:crossAx val="912690"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75328291"/>
+        <c:axId val="912690"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2343,7 +2740,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13500643"/>
+        <c:crossAx val="79649927"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2380,7 +2777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2682,11 +3079,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55276602"/>
-        <c:axId val="64867288"/>
+        <c:axId val="13541174"/>
+        <c:axId val="2025595"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55276602"/>
+        <c:axId val="13541174"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,11 +3099,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64867288"/>
+        <c:crossAx val="2025595"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64867288"/>
+        <c:axId val="2025595"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2731,7 +3128,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55276602"/>
+        <c:crossAx val="13541174"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2768,7 +3165,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3070,11 +3467,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="4911865"/>
-        <c:axId val="88081329"/>
+        <c:axId val="85083678"/>
+        <c:axId val="82552179"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4911865"/>
+        <c:axId val="85083678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3090,11 +3487,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88081329"/>
+        <c:crossAx val="82552179"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88081329"/>
+        <c:axId val="82552179"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3119,7 +3516,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4911865"/>
+        <c:crossAx val="85083678"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3156,7 +3553,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3458,11 +3855,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="5491030"/>
-        <c:axId val="45978526"/>
+        <c:axId val="11492457"/>
+        <c:axId val="6576215"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5491030"/>
+        <c:axId val="11492457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3478,11 +3875,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45978526"/>
+        <c:crossAx val="6576215"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45978526"/>
+        <c:axId val="6576215"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3507,7 +3904,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5491030"/>
+        <c:crossAx val="11492457"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3544,7 +3941,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3846,11 +4243,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93550089"/>
-        <c:axId val="20350263"/>
+        <c:axId val="89868817"/>
+        <c:axId val="73376911"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93550089"/>
+        <c:axId val="89868817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3866,11 +4263,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20350263"/>
+        <c:crossAx val="73376911"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20350263"/>
+        <c:axId val="73376911"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3895,395 +4292,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93550089"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:solidFill>
-        <a:srgbClr val="808080"/>
-      </a:solidFill>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>rate Fe red</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>exponential</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="666699"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="666699"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>89.6908203872887</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80.8537071093311</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41.3625242918782</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.8160678720006</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.93288575140178</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.123403969229771</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>linear</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="993366"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="993366"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>76.4442340767933</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80.8518175958458</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62.9572589474022</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59.3976979843909</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39.933770521939</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18.2777936214685</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>no</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="99cc00"/>
-            </a:solidFill>
-            <a:ln w="25200">
-              <a:solidFill>
-                <a:srgbClr val="99cc00"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.3237456245636E-007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.73617866144958E-007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8643376671461E-007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.49892067269166E-007</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.26312960937686E-007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.20473261085559E-007</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="35356167"/>
-        <c:axId val="48121943"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="35356167"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="808080"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="48121943"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="48121943"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="808080"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="808080"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="35356167"/>
+        <c:crossAx val="89868817"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4325,15 +4334,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>306360</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>625680</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:colOff>652320</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4341,8 +4350,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="306360" y="18080640"/>
-        <a:ext cx="5072760" cy="2890080"/>
+        <a:off x="333360" y="18066240"/>
+        <a:ext cx="5072400" cy="2886840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4355,15 +4364,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>587880</xdr:colOff>
+      <xdr:colOff>615240</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>294120</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4371,8 +4380,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6416280" y="18071280"/>
-        <a:ext cx="6783840" cy="2890080"/>
+        <a:off x="6443640" y="18056880"/>
+        <a:ext cx="7182000" cy="2886840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4385,15 +4394,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>455760</xdr:colOff>
+      <xdr:colOff>482400</xdr:colOff>
       <xdr:row>144</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4401,8 +4410,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="108000" y="21171960"/>
-        <a:ext cx="8972280" cy="2766960"/>
+        <a:off x="135000" y="21155040"/>
+        <a:ext cx="8971920" cy="2766240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4415,15 +4424,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>442800</xdr:colOff>
+      <xdr:colOff>469800</xdr:colOff>
       <xdr:row>126</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>762120</xdr:colOff>
+      <xdr:colOff>788760</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4431,8 +4440,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9683280" y="21119760"/>
-        <a:ext cx="5702760" cy="2743560"/>
+        <a:off x="9710280" y="21102840"/>
+        <a:ext cx="6101280" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4445,15 +4454,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>707760</xdr:colOff>
+      <xdr:colOff>735120</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>703800</xdr:colOff>
+      <xdr:colOff>730440</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4461,8 +4470,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13640760" y="18047880"/>
-        <a:ext cx="5394600" cy="2721960"/>
+        <a:off x="14066640" y="18033480"/>
+        <a:ext cx="5394240" cy="2718720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4475,15 +4484,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>426960</xdr:colOff>
+      <xdr:colOff>453600</xdr:colOff>
       <xdr:row>163</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4491,8 +4500,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="108000" y="24315480"/>
-        <a:ext cx="5072400" cy="2726280"/>
+        <a:off x="135000" y="24298560"/>
+        <a:ext cx="5072040" cy="2725560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4505,15 +4514,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>259200</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:colOff>286560</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>577440</xdr:colOff>
+      <xdr:colOff>604080</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4521,8 +4530,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6087600" y="24217200"/>
-        <a:ext cx="6488640" cy="2719800"/>
+        <a:off x="6114960" y="24200280"/>
+        <a:ext cx="6886800" cy="2719080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4535,15 +4544,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>159120</xdr:colOff>
+      <xdr:colOff>186480</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>969120</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:colOff>995760</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4551,8 +4560,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13092120" y="24245640"/>
-        <a:ext cx="7338960" cy="2719800"/>
+        <a:off x="13518000" y="24228720"/>
+        <a:ext cx="7338600" cy="2719080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4565,15 +4574,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
-      <xdr:row>164</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:colOff>284400</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
+      <xdr:colOff>603360</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4581,8 +4590,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="257400" y="27293760"/>
-        <a:ext cx="5072760" cy="2719440"/>
+        <a:off x="284400" y="27276840"/>
+        <a:ext cx="5072400" cy="2719080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4595,15 +4604,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>259200</xdr:colOff>
-      <xdr:row>164</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:colOff>286560</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>577440</xdr:colOff>
+      <xdr:colOff>604080</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4611,8 +4620,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6087600" y="27293760"/>
-        <a:ext cx="6488640" cy="2719440"/>
+        <a:off x="6114960" y="27276840"/>
+        <a:ext cx="6886800" cy="2719080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4632,8 +4641,8 @@
   </sheetPr>
   <dimension ref="A1:AD126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4642,7 +4651,8 @@
     <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.8163265306122"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.234693877551"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.3826530612245"/>
     <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.8163265306122"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2397959183673"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.234693877551"/>
@@ -4660,7 +4670,7 @@
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4697,8 +4707,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="N1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,15 +4751,19 @@
       <c r="L2" s="1" t="n">
         <v>89.6908203872887</v>
       </c>
+      <c r="M2" s="2" t="n">
+        <f aca="false">H2+I2+J2+K2+L2</f>
+        <v>360.519530928432</v>
+      </c>
       <c r="N2" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A2)</f>
         <v>510.23765402814</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,21 +4803,25 @@
       <c r="L3" s="1" t="n">
         <v>80.8537071093311</v>
       </c>
+      <c r="M3" s="2" t="n">
+        <f aca="false">H3+I3+J3+K3+L3</f>
+        <v>322.755834108843</v>
+      </c>
       <c r="N3" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A3)</f>
         <v>466.52240423087</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4840,15 +4861,19 @@
       <c r="L4" s="1" t="n">
         <v>41.3625242918782</v>
       </c>
+      <c r="M4" s="2" t="n">
+        <f aca="false">H4+I4+J4+K4+L4</f>
+        <v>229.409072881492</v>
+      </c>
       <c r="N4" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A4)</f>
         <v>356.592746676823</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W4" s="0" t="n">
         <f aca="false">38*365*1000/100^2</f>
@@ -4900,12 +4925,16 @@
       <c r="L5" s="1" t="n">
         <v>17.8160678720006</v>
       </c>
+      <c r="M5" s="2" t="n">
+        <f aca="false">H5+I5+J5+K5+L5</f>
+        <v>141.794098441373</v>
+      </c>
       <c r="N5" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A5)</f>
         <v>227.862314874044</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>0.17</v>
@@ -4954,12 +4983,16 @@
       <c r="L6" s="1" t="n">
         <v>1.93288575140178</v>
       </c>
+      <c r="M6" s="2" t="n">
+        <f aca="false">H6+I6+J6+K6+L6</f>
+        <v>56.5405057425002</v>
+      </c>
       <c r="N6" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A6)</f>
         <v>93.0406005777163</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="W6" s="0" t="n">
         <v>0.018</v>
@@ -5008,15 +5041,19 @@
       <c r="L7" s="1" t="n">
         <v>0.123403969229771</v>
       </c>
+      <c r="M7" s="2" t="n">
+        <f aca="false">H7+I7+J7+K7+L7</f>
+        <v>17.0123034856124</v>
+      </c>
       <c r="N7" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A7)</f>
         <v>24.2757415470021</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W7" s="0" t="n">
         <v>0.00046</v>
@@ -5065,50 +5102,54 @@
       <c r="L8" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="M8" s="2" t="n">
+        <f aca="false">H8+I8+J8+K8+L8</f>
+        <v>6.20949318022361</v>
+      </c>
       <c r="N8" s="0" t="n">
         <f aca="false">1800*10^(-0.5086-0.000389*A8)</f>
         <v>6.33391899877725</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="0" t="n">
         <v>100</v>
@@ -5165,6 +5206,13 @@
         <f aca="false">B2/G2</f>
         <v>0.383476645926384</v>
       </c>
+      <c r="L10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <f aca="false">M2/M8</f>
+        <v>58.0594132990817</v>
+      </c>
       <c r="Q10" s="0" t="n">
         <v>200</v>
       </c>
@@ -5498,27 +5546,27 @@
     </row>
     <row r="18" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -5539,10 +5587,10 @@
         <v>9</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>1</v>
@@ -5563,7 +5611,7 @@
         <v>9</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5939,28 +5987,30 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S29" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1</v>
@@ -5981,10 +6031,10 @@
         <v>9</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>1</v>
@@ -6005,9 +6055,20 @@
         <v>9</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="S30" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V30" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="n">
@@ -6058,7 +6119,14 @@
       <c r="Q31" s="4" t="n">
         <v>-0.00276497202706358</v>
       </c>
-      <c r="S31" s="9"/>
+      <c r="S31" s="9" t="n">
+        <f aca="false">B31/K31</f>
+        <v>8.95227596776428</v>
+      </c>
+      <c r="V31" s="0" t="n">
+        <f aca="false">Q31/Q37</f>
+        <v>15.7855273111069</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="n">
@@ -6109,7 +6177,10 @@
       <c r="Q32" s="4" t="n">
         <v>-0.00265084299362961</v>
       </c>
-      <c r="S32" s="9"/>
+      <c r="S32" s="9" t="n">
+        <f aca="false">B32/K32</f>
+        <v>8.7620765466953</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="n">
@@ -6160,7 +6231,10 @@
       <c r="Q33" s="4" t="n">
         <v>-0.00172199278884368</v>
       </c>
-      <c r="S33" s="9"/>
+      <c r="S33" s="9" t="n">
+        <f aca="false">B33/K33</f>
+        <v>7.24084876576374</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="n">
@@ -6211,7 +6285,10 @@
       <c r="Q34" s="4" t="n">
         <v>-0.00135442138713308</v>
       </c>
-      <c r="S34" s="9"/>
+      <c r="S34" s="9" t="n">
+        <f aca="false">B34/K34</f>
+        <v>6.20036769519386</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="n">
@@ -6262,7 +6339,10 @@
       <c r="Q35" s="4" t="n">
         <v>-0.000806616866194659</v>
       </c>
-      <c r="S35" s="9"/>
+      <c r="S35" s="9" t="n">
+        <f aca="false">B35/K35</f>
+        <v>4.10370222060546</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="n">
@@ -6313,7 +6393,10 @@
       <c r="Q36" s="4" t="n">
         <v>-0.000369702830443225</v>
       </c>
-      <c r="S36" s="9"/>
+      <c r="S36" s="9" t="n">
+        <f aca="false">B36/K36</f>
+        <v>1.98428078203995</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="n">
@@ -6364,7 +6447,10 @@
       <c r="Q37" s="4" t="n">
         <v>-0.000175158673674342</v>
       </c>
-      <c r="S37" s="9"/>
+      <c r="S37" s="9" t="n">
+        <f aca="false">B37/K37</f>
+        <v>1.20630372782124</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
@@ -6372,28 +6458,28 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>1</v>
@@ -6414,10 +6500,10 @@
         <v>9</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>1</v>
@@ -6438,7 +6524,7 @@
         <v>9</v>
       </c>
       <c r="Q40" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S40" s="9"/>
     </row>
@@ -6686,28 +6772,28 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="S50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>1</v>
@@ -6728,10 +6814,10 @@
         <v>9</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>1</v>
@@ -6752,7 +6838,7 @@
         <v>9</v>
       </c>
       <c r="Q51" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S51" s="9"/>
     </row>
@@ -6999,27 +7085,27 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>1</v>
@@ -7040,10 +7126,10 @@
         <v>9</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>1</v>
@@ -7064,7 +7150,7 @@
         <v>9</v>
       </c>
       <c r="Q61" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7169,27 +7255,27 @@
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>1</v>
@@ -7210,10 +7296,10 @@
         <v>9</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>1</v>
@@ -7234,7 +7320,7 @@
         <v>9</v>
       </c>
       <c r="Q71" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7341,27 +7427,27 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>1</v>
@@ -7382,10 +7468,10 @@
         <v>9</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>1</v>
@@ -7406,7 +7492,7 @@
         <v>9</v>
       </c>
       <c r="Q81" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7482,27 +7568,27 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K91" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>1</v>
@@ -7523,10 +7609,10 @@
         <v>9</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>1</v>
@@ -7547,7 +7633,7 @@
         <v>9</v>
       </c>
       <c r="Q92" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,13 +7772,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -7704,19 +7790,19 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8022,13 +8108,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -8040,19 +8126,19 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>